<commit_message>
Move checkpoint data to transformed folder
</commit_message>
<xml_diff>
--- a/data/raw/dosm-number_of_crime_by_state-2015-2018.xlsx
+++ b/data/raw/dosm-number_of_crime_by_state-2015-2018.xlsx
@@ -1,58 +1,68 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\GitHub\time-series-house-price-forecasting\data\raw\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9218621-B654-4201-8479-BD2B054D99D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="11715" windowHeight="9120"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Violent Crime by Contingent, PD" sheetId="1" r:id="rId3"/>
+    <sheet name="Violent Crime by Contingent, PD" sheetId="1" r:id="rId1"/>
+    <sheet name="Transformed" sheetId="2" r:id="rId2"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>Violent Crime by Contingent, PDRM District and Type of Crime, Malaysia, 2015-2018</t>
   </si>
   <si>
-    <t xml:space="preserve">State</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Number Of Crime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Year</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contingent PDRM District</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Causing injury</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rape</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robbery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">W.P. Kuala Lumpur</t>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Number Of Crime</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>Contingent PDRM District</t>
+  </si>
+  <si>
+    <t>Causing injury</t>
+  </si>
+  <si>
+    <t>Murder</t>
+  </si>
+  <si>
+    <t>Rape</t>
+  </si>
+  <si>
+    <t>Robbery</t>
+  </si>
+  <si>
+    <t>W.P. Kuala Lumpur</t>
   </si>
   <si>
     <t xml:space="preserve">Brickfields </t>
@@ -70,17 +80,20 @@
     <t xml:space="preserve">Wangsa Maju </t>
   </si>
   <si>
-    <t xml:space="preserve">Total</t>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Crime Type</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="#,##0_);(#,##0)"/>
+    <numFmt numFmtId="164" formatCode="#,##0_);\(#,##0\)"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -98,7 +111,7 @@
       <name val="Arial Narrow"/>
     </font>
     <font>
-      <u val="single"/>
+      <u/>
       <sz val="11"/>
       <color rgb="FF35383A"/>
       <name val="Arial Narrow"/>
@@ -109,13 +122,17 @@
       <color rgb="FFFFFFFF"/>
       <name val="Arial Narrow"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -138,47 +155,64 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
-      <left>
-        <color rgb="FFEBEBEB"/>
-      </left>
-      <right style="thin"/>
-      <top>
-        <color rgb="FFEBEBEB"/>
-      </top>
-      <bottom style="thin"/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left>
-        <color rgb="FFEBEBEB"/>
-      </left>
+      <left/>
       <right style="thin">
         <color rgb="FF35383A"/>
       </right>
-      <top>
-        <color rgb="FFEBEBEB"/>
-      </top>
+      <top/>
       <bottom style="thin">
         <color rgb="FF35383A"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF35383A"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF35383A"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF35383A"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="bottom" wrapText="0"/>
-    </xf>
+  <cellXfs count="16">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="0"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -186,117 +220,433 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="0"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="0"/>
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/worksheets/worksheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.57142857" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="10.85714286" customWidth="1"/>
-    <col min="4" max="4" width="10.85714286" customWidth="1"/>
-    <col min="5" max="5" width="10.85714286" customWidth="1"/>
-    <col min="6" max="6" width="10.85714286" customWidth="1"/>
-    <col min="7" max="7" width="10.85714286" customWidth="1"/>
-    <col min="8" max="8" width="10.85714286" customWidth="1"/>
-    <col min="9" max="9" width="10.85714286" customWidth="1"/>
-    <col min="10" max="10" width="10.85714286" customWidth="1"/>
-    <col min="11" max="11" width="10.85714286" customWidth="1"/>
-    <col min="12" max="12" width="10.85714286" customWidth="1"/>
-    <col min="13" max="13" width="10.85714286" customWidth="1"/>
-    <col min="14" max="14" width="10.85714286" customWidth="1"/>
-    <col min="15" max="15" width="10.85714286" customWidth="1"/>
-    <col min="16" max="16" width="10.85714286" customWidth="1"/>
-    <col min="17" max="17" width="10.85714286" customWidth="1"/>
-    <col min="18" max="18" width="10.85714286" customWidth="1"/>
+    <col min="3" max="18" width="10.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s"/>
-      <c r="C3" s="2" t="s">
+      <c r="B3" s="2"/>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="2"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+    </row>
+    <row r="4" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9"/>
       <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2" t="s">
+      <c r="L4" s="9"/>
+      <c r="M4" s="9"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9"/>
+    </row>
+    <row r="5" spans="1:18" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -349,8 +699,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -405,8 +755,8 @@
         <v>324</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="10"/>
       <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
@@ -459,8 +809,8 @@
         <v>176</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" s="3"/>
+    <row r="8" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
@@ -513,8 +863,8 @@
         <v>1211</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="3"/>
+    <row r="9" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="10"/>
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
@@ -567,8 +917,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" s="3"/>
+    <row r="10" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="10"/>
       <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
@@ -621,11 +971,11 @@
         <v>460</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:18" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="7" t="s"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="8">
         <v>716</v>
       </c>
@@ -677,13 +1027,457 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A6:A10"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="C3:R3"/>
     <mergeCell ref="C4:F4"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="K4:N4"/>
     <mergeCell ref="O4:R4"/>
-    <mergeCell ref="A6:A10"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E422775-3976-48C5-A476-2299BE618C0D}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="4">
+        <v>108</v>
+      </c>
+      <c r="D2" s="6">
+        <v>85</v>
+      </c>
+      <c r="E2" s="4">
+        <v>189</v>
+      </c>
+      <c r="F2" s="6">
+        <v>244</v>
+      </c>
+      <c r="G2" s="4">
+        <v>90</v>
+      </c>
+      <c r="H2" s="8">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4">
+        <v>9</v>
+      </c>
+      <c r="F3" s="6">
+        <v>11</v>
+      </c>
+      <c r="G3" s="4">
+        <v>5</v>
+      </c>
+      <c r="H3" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="4">
+        <v>16</v>
+      </c>
+      <c r="D4" s="6">
+        <v>33</v>
+      </c>
+      <c r="E4" s="4">
+        <v>22</v>
+      </c>
+      <c r="F4" s="6">
+        <v>24</v>
+      </c>
+      <c r="G4" s="4">
+        <v>24</v>
+      </c>
+      <c r="H4" s="8">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9"/>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="4">
+        <v>471</v>
+      </c>
+      <c r="D5" s="6">
+        <v>438</v>
+      </c>
+      <c r="E5" s="4">
+        <v>781</v>
+      </c>
+      <c r="F5" s="6">
+        <v>613</v>
+      </c>
+      <c r="G5" s="4">
+        <v>473</v>
+      </c>
+      <c r="H5" s="8">
+        <v>2776</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="4">
+        <v>54</v>
+      </c>
+      <c r="D6" s="6">
+        <v>89</v>
+      </c>
+      <c r="E6" s="4">
+        <v>201</v>
+      </c>
+      <c r="F6" s="6">
+        <v>175</v>
+      </c>
+      <c r="G6" s="4">
+        <v>120</v>
+      </c>
+      <c r="H6" s="8">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9"/>
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6</v>
+      </c>
+      <c r="F7" s="6">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4">
+        <v>7</v>
+      </c>
+      <c r="H7" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4">
+        <v>13</v>
+      </c>
+      <c r="D8" s="6">
+        <v>8</v>
+      </c>
+      <c r="E8" s="4">
+        <v>25</v>
+      </c>
+      <c r="F8" s="6">
+        <v>24</v>
+      </c>
+      <c r="G8" s="4">
+        <v>18</v>
+      </c>
+      <c r="H8" s="8">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9"/>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4">
+        <v>536</v>
+      </c>
+      <c r="D9" s="6">
+        <v>354</v>
+      </c>
+      <c r="E9" s="4">
+        <v>829</v>
+      </c>
+      <c r="F9" s="6">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4">
+        <v>700</v>
+      </c>
+      <c r="H9" s="8">
+        <v>2434</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="4">
+        <v>69</v>
+      </c>
+      <c r="D10" s="6">
+        <v>83</v>
+      </c>
+      <c r="E10" s="4">
+        <v>161</v>
+      </c>
+      <c r="F10" s="6">
+        <v>201</v>
+      </c>
+      <c r="G10" s="4">
+        <v>134</v>
+      </c>
+      <c r="H10" s="8">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9"/>
+      <c r="B11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="6">
+        <v>5</v>
+      </c>
+      <c r="E11" s="4">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>15</v>
+      </c>
+      <c r="G11" s="4">
+        <v>5</v>
+      </c>
+      <c r="H11" s="8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9"/>
+      <c r="B12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="4">
+        <v>24</v>
+      </c>
+      <c r="D12" s="6">
+        <v>23</v>
+      </c>
+      <c r="E12" s="4">
+        <v>30</v>
+      </c>
+      <c r="F12" s="6">
+        <v>21</v>
+      </c>
+      <c r="G12" s="4">
+        <v>32</v>
+      </c>
+      <c r="H12" s="8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <v>484</v>
+      </c>
+      <c r="D13" s="6">
+        <v>361</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1151</v>
+      </c>
+      <c r="F13" s="6">
+        <v>14</v>
+      </c>
+      <c r="G13" s="4">
+        <v>547</v>
+      </c>
+      <c r="H13" s="8">
+        <v>2557</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="4">
+        <v>71</v>
+      </c>
+      <c r="D14" s="6">
+        <v>73</v>
+      </c>
+      <c r="E14" s="4">
+        <v>112</v>
+      </c>
+      <c r="F14" s="6">
+        <v>163</v>
+      </c>
+      <c r="G14" s="4">
+        <v>95</v>
+      </c>
+      <c r="H14" s="8">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="4">
+        <v>3</v>
+      </c>
+      <c r="D15" s="6">
+        <v>3</v>
+      </c>
+      <c r="E15" s="4">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6">
+        <v>12</v>
+      </c>
+      <c r="G15" s="4">
+        <v>7</v>
+      </c>
+      <c r="H15" s="8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="4">
+        <v>20</v>
+      </c>
+      <c r="D16" s="6">
+        <v>27</v>
+      </c>
+      <c r="E16" s="4">
+        <v>23</v>
+      </c>
+      <c r="F16" s="6">
+        <v>24</v>
+      </c>
+      <c r="G16" s="4">
+        <v>16</v>
+      </c>
+      <c r="H16" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="4">
+        <v>324</v>
+      </c>
+      <c r="D17" s="6">
+        <v>176</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1211</v>
+      </c>
+      <c r="F17" s="6">
+        <v>9</v>
+      </c>
+      <c r="G17" s="4">
+        <v>460</v>
+      </c>
+      <c r="H17" s="8">
+        <v>2180</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+  </mergeCells>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>